<commit_message>
VV VW working (the pDampCoef needs to be small less than 0.25 in this case)
</commit_message>
<xml_diff>
--- a/ProjectFiles/HECO/PyDSS Settings/HP-VV-VW-R/pyControllerList/PV Controller.xlsx
+++ b/ProjectFiles/HECO/PyDSS Settings/HP-VV-VW-R/pyControllerList/PV Controller.xlsx
@@ -2864,8 +2864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y533"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3079,7 +3079,7 @@
         <v>564</v>
       </c>
       <c r="X3" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y3" s="4">
         <v>0.7</v>
@@ -3156,7 +3156,7 @@
         <v>564</v>
       </c>
       <c r="X4" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y4" s="4">
         <v>0.7</v>
@@ -3233,7 +3233,7 @@
         <v>564</v>
       </c>
       <c r="X5" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y5" s="4">
         <v>0.7</v>
@@ -3310,7 +3310,7 @@
         <v>564</v>
       </c>
       <c r="X6" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y6" s="4">
         <v>0.7</v>
@@ -3387,7 +3387,7 @@
         <v>564</v>
       </c>
       <c r="X7" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y7" s="4">
         <v>0.7</v>
@@ -3464,7 +3464,7 @@
         <v>564</v>
       </c>
       <c r="X8" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y8" s="4">
         <v>0.7</v>
@@ -3541,7 +3541,7 @@
         <v>564</v>
       </c>
       <c r="X9" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y9" s="4">
         <v>0.7</v>
@@ -3618,7 +3618,7 @@
         <v>564</v>
       </c>
       <c r="X10" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y10" s="4">
         <v>0.7</v>
@@ -3695,7 +3695,7 @@
         <v>564</v>
       </c>
       <c r="X11" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y11" s="4">
         <v>0.7</v>
@@ -3772,7 +3772,7 @@
         <v>564</v>
       </c>
       <c r="X12" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y12" s="4">
         <v>0.7</v>
@@ -3849,7 +3849,7 @@
         <v>564</v>
       </c>
       <c r="X13" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y13" s="4">
         <v>0.7</v>
@@ -3926,7 +3926,7 @@
         <v>564</v>
       </c>
       <c r="X14" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y14" s="4">
         <v>0.7</v>
@@ -4003,7 +4003,7 @@
         <v>564</v>
       </c>
       <c r="X15" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y15" s="4">
         <v>0.7</v>
@@ -4080,7 +4080,7 @@
         <v>564</v>
       </c>
       <c r="X16" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y16" s="4">
         <v>0.7</v>
@@ -4157,7 +4157,7 @@
         <v>564</v>
       </c>
       <c r="X17" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y17" s="4">
         <v>0.7</v>
@@ -4234,7 +4234,7 @@
         <v>564</v>
       </c>
       <c r="X18" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y18" s="4">
         <v>0.7</v>
@@ -4311,7 +4311,7 @@
         <v>564</v>
       </c>
       <c r="X19" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y19" s="4">
         <v>0.7</v>
@@ -4388,7 +4388,7 @@
         <v>564</v>
       </c>
       <c r="X20" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y20" s="4">
         <v>0.7</v>
@@ -4465,7 +4465,7 @@
         <v>564</v>
       </c>
       <c r="X21" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y21" s="4">
         <v>0.7</v>
@@ -4542,7 +4542,7 @@
         <v>564</v>
       </c>
       <c r="X22" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y22" s="4">
         <v>0.7</v>
@@ -4619,7 +4619,7 @@
         <v>564</v>
       </c>
       <c r="X23" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y23" s="4">
         <v>0.7</v>
@@ -4696,7 +4696,7 @@
         <v>564</v>
       </c>
       <c r="X24" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y24" s="4">
         <v>0.7</v>
@@ -4773,7 +4773,7 @@
         <v>564</v>
       </c>
       <c r="X25" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y25" s="4">
         <v>0.7</v>
@@ -4850,7 +4850,7 @@
         <v>564</v>
       </c>
       <c r="X26" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y26" s="4">
         <v>0.7</v>
@@ -4927,7 +4927,7 @@
         <v>564</v>
       </c>
       <c r="X27" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y27" s="4">
         <v>0.7</v>
@@ -5004,7 +5004,7 @@
         <v>564</v>
       </c>
       <c r="X28" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y28" s="4">
         <v>0.7</v>
@@ -5081,7 +5081,7 @@
         <v>564</v>
       </c>
       <c r="X29" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y29" s="4">
         <v>0.7</v>
@@ -5158,7 +5158,7 @@
         <v>564</v>
       </c>
       <c r="X30" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y30" s="4">
         <v>0.7</v>
@@ -5235,7 +5235,7 @@
         <v>564</v>
       </c>
       <c r="X31" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y31" s="4">
         <v>0.7</v>
@@ -5312,7 +5312,7 @@
         <v>564</v>
       </c>
       <c r="X32" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y32" s="4">
         <v>0.7</v>
@@ -5389,7 +5389,7 @@
         <v>564</v>
       </c>
       <c r="X33" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y33" s="4">
         <v>0.7</v>
@@ -5466,7 +5466,7 @@
         <v>564</v>
       </c>
       <c r="X34" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y34" s="4">
         <v>0.7</v>
@@ -5543,7 +5543,7 @@
         <v>564</v>
       </c>
       <c r="X35" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y35" s="4">
         <v>0.7</v>
@@ -5620,7 +5620,7 @@
         <v>564</v>
       </c>
       <c r="X36" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y36" s="4">
         <v>0.7</v>
@@ -5697,7 +5697,7 @@
         <v>564</v>
       </c>
       <c r="X37" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y37" s="4">
         <v>0.7</v>
@@ -5774,7 +5774,7 @@
         <v>564</v>
       </c>
       <c r="X38" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y38" s="4">
         <v>0.7</v>
@@ -5851,7 +5851,7 @@
         <v>564</v>
       </c>
       <c r="X39" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y39" s="4">
         <v>0.7</v>
@@ -5928,7 +5928,7 @@
         <v>564</v>
       </c>
       <c r="X40" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y40" s="4">
         <v>0.7</v>
@@ -6005,7 +6005,7 @@
         <v>564</v>
       </c>
       <c r="X41" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y41" s="4">
         <v>0.7</v>
@@ -6082,7 +6082,7 @@
         <v>564</v>
       </c>
       <c r="X42" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y42" s="4">
         <v>0.7</v>
@@ -6159,7 +6159,7 @@
         <v>564</v>
       </c>
       <c r="X43" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y43" s="4">
         <v>0.7</v>
@@ -6236,7 +6236,7 @@
         <v>564</v>
       </c>
       <c r="X44" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y44" s="4">
         <v>0.7</v>
@@ -6313,7 +6313,7 @@
         <v>564</v>
       </c>
       <c r="X45" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y45" s="4">
         <v>0.7</v>
@@ -6390,7 +6390,7 @@
         <v>564</v>
       </c>
       <c r="X46" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y46" s="4">
         <v>0.7</v>
@@ -6467,7 +6467,7 @@
         <v>564</v>
       </c>
       <c r="X47" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y47" s="4">
         <v>0.7</v>
@@ -6544,7 +6544,7 @@
         <v>564</v>
       </c>
       <c r="X48" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y48" s="4">
         <v>0.7</v>
@@ -6621,7 +6621,7 @@
         <v>564</v>
       </c>
       <c r="X49" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y49" s="4">
         <v>0.7</v>
@@ -6698,7 +6698,7 @@
         <v>564</v>
       </c>
       <c r="X50" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y50" s="4">
         <v>0.7</v>
@@ -6775,7 +6775,7 @@
         <v>564</v>
       </c>
       <c r="X51" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y51" s="4">
         <v>0.7</v>
@@ -6852,7 +6852,7 @@
         <v>564</v>
       </c>
       <c r="X52" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y52" s="4">
         <v>0.7</v>
@@ -6929,7 +6929,7 @@
         <v>564</v>
       </c>
       <c r="X53" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y53" s="4">
         <v>0.7</v>
@@ -7006,7 +7006,7 @@
         <v>564</v>
       </c>
       <c r="X54" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y54" s="4">
         <v>0.7</v>
@@ -7083,7 +7083,7 @@
         <v>564</v>
       </c>
       <c r="X55" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y55" s="4">
         <v>0.7</v>
@@ -7160,7 +7160,7 @@
         <v>564</v>
       </c>
       <c r="X56" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y56" s="4">
         <v>0.7</v>
@@ -7237,7 +7237,7 @@
         <v>564</v>
       </c>
       <c r="X57" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y57" s="4">
         <v>0.7</v>
@@ -7314,7 +7314,7 @@
         <v>564</v>
       </c>
       <c r="X58" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y58" s="4">
         <v>0.7</v>
@@ -7391,7 +7391,7 @@
         <v>564</v>
       </c>
       <c r="X59" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y59" s="4">
         <v>0.7</v>
@@ -7468,7 +7468,7 @@
         <v>564</v>
       </c>
       <c r="X60" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y60" s="4">
         <v>0.7</v>
@@ -7545,7 +7545,7 @@
         <v>564</v>
       </c>
       <c r="X61" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y61" s="4">
         <v>0.7</v>
@@ -7622,7 +7622,7 @@
         <v>564</v>
       </c>
       <c r="X62" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y62" s="4">
         <v>0.7</v>
@@ -7699,7 +7699,7 @@
         <v>564</v>
       </c>
       <c r="X63" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y63" s="4">
         <v>0.7</v>
@@ -7776,7 +7776,7 @@
         <v>564</v>
       </c>
       <c r="X64" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y64" s="4">
         <v>0.7</v>
@@ -7853,7 +7853,7 @@
         <v>564</v>
       </c>
       <c r="X65" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y65" s="4">
         <v>0.7</v>
@@ -7930,7 +7930,7 @@
         <v>564</v>
       </c>
       <c r="X66" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y66" s="4">
         <v>0.7</v>
@@ -8007,7 +8007,7 @@
         <v>564</v>
       </c>
       <c r="X67" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y67" s="4">
         <v>0.7</v>
@@ -8084,7 +8084,7 @@
         <v>564</v>
       </c>
       <c r="X68" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y68" s="4">
         <v>0.7</v>
@@ -8161,7 +8161,7 @@
         <v>564</v>
       </c>
       <c r="X69" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y69" s="4">
         <v>0.7</v>
@@ -8238,7 +8238,7 @@
         <v>564</v>
       </c>
       <c r="X70" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y70" s="4">
         <v>0.7</v>
@@ -8315,7 +8315,7 @@
         <v>564</v>
       </c>
       <c r="X71" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y71" s="4">
         <v>0.7</v>
@@ -8392,7 +8392,7 @@
         <v>564</v>
       </c>
       <c r="X72" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y72" s="4">
         <v>0.7</v>
@@ -8469,7 +8469,7 @@
         <v>564</v>
       </c>
       <c r="X73" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y73" s="4">
         <v>0.7</v>
@@ -8546,7 +8546,7 @@
         <v>564</v>
       </c>
       <c r="X74" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y74" s="4">
         <v>0.7</v>
@@ -8623,7 +8623,7 @@
         <v>564</v>
       </c>
       <c r="X75" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y75" s="4">
         <v>0.7</v>
@@ -8700,7 +8700,7 @@
         <v>564</v>
       </c>
       <c r="X76" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y76" s="4">
         <v>0.7</v>
@@ -8777,7 +8777,7 @@
         <v>564</v>
       </c>
       <c r="X77" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y77" s="4">
         <v>0.7</v>
@@ -8854,7 +8854,7 @@
         <v>564</v>
       </c>
       <c r="X78" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y78" s="4">
         <v>0.7</v>
@@ -8931,7 +8931,7 @@
         <v>564</v>
       </c>
       <c r="X79" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y79" s="4">
         <v>0.7</v>
@@ -9008,7 +9008,7 @@
         <v>564</v>
       </c>
       <c r="X80" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y80" s="4">
         <v>0.7</v>
@@ -9085,7 +9085,7 @@
         <v>564</v>
       </c>
       <c r="X81" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y81" s="4">
         <v>0.7</v>
@@ -9162,7 +9162,7 @@
         <v>564</v>
       </c>
       <c r="X82" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y82" s="4">
         <v>0.7</v>
@@ -9239,7 +9239,7 @@
         <v>564</v>
       </c>
       <c r="X83" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y83" s="4">
         <v>0.7</v>
@@ -9316,7 +9316,7 @@
         <v>564</v>
       </c>
       <c r="X84" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y84" s="4">
         <v>0.7</v>
@@ -9393,7 +9393,7 @@
         <v>564</v>
       </c>
       <c r="X85" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y85" s="4">
         <v>0.7</v>
@@ -9470,7 +9470,7 @@
         <v>564</v>
       </c>
       <c r="X86" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y86" s="4">
         <v>0.7</v>
@@ -9547,7 +9547,7 @@
         <v>564</v>
       </c>
       <c r="X87" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y87" s="4">
         <v>0.7</v>
@@ -9624,7 +9624,7 @@
         <v>564</v>
       </c>
       <c r="X88" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y88" s="4">
         <v>0.7</v>
@@ -9701,7 +9701,7 @@
         <v>564</v>
       </c>
       <c r="X89" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y89" s="4">
         <v>0.7</v>
@@ -9778,7 +9778,7 @@
         <v>564</v>
       </c>
       <c r="X90" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y90" s="4">
         <v>0.7</v>
@@ -9855,7 +9855,7 @@
         <v>564</v>
       </c>
       <c r="X91" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y91" s="4">
         <v>0.7</v>
@@ -9932,7 +9932,7 @@
         <v>564</v>
       </c>
       <c r="X92" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y92" s="4">
         <v>0.7</v>
@@ -10009,7 +10009,7 @@
         <v>564</v>
       </c>
       <c r="X93" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y93" s="4">
         <v>0.7</v>
@@ -10086,7 +10086,7 @@
         <v>564</v>
       </c>
       <c r="X94" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y94" s="4">
         <v>0.7</v>
@@ -10163,7 +10163,7 @@
         <v>564</v>
       </c>
       <c r="X95" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y95" s="4">
         <v>0.7</v>
@@ -10240,7 +10240,7 @@
         <v>564</v>
       </c>
       <c r="X96" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y96" s="4">
         <v>0.7</v>
@@ -10317,7 +10317,7 @@
         <v>564</v>
       </c>
       <c r="X97" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y97" s="4">
         <v>0.7</v>
@@ -10394,7 +10394,7 @@
         <v>564</v>
       </c>
       <c r="X98" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y98" s="4">
         <v>0.7</v>
@@ -10471,7 +10471,7 @@
         <v>564</v>
       </c>
       <c r="X99" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y99" s="4">
         <v>0.7</v>
@@ -10548,7 +10548,7 @@
         <v>564</v>
       </c>
       <c r="X100" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y100" s="4">
         <v>0.7</v>
@@ -10625,7 +10625,7 @@
         <v>564</v>
       </c>
       <c r="X101" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y101" s="4">
         <v>0.7</v>
@@ -10702,7 +10702,7 @@
         <v>564</v>
       </c>
       <c r="X102" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y102" s="4">
         <v>0.7</v>
@@ -10779,7 +10779,7 @@
         <v>564</v>
       </c>
       <c r="X103" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y103" s="4">
         <v>0.7</v>
@@ -10856,7 +10856,7 @@
         <v>564</v>
       </c>
       <c r="X104" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y104" s="4">
         <v>0.7</v>
@@ -10933,7 +10933,7 @@
         <v>564</v>
       </c>
       <c r="X105" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y105" s="4">
         <v>0.7</v>
@@ -11010,7 +11010,7 @@
         <v>564</v>
       </c>
       <c r="X106" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y106" s="4">
         <v>0.7</v>
@@ -11087,7 +11087,7 @@
         <v>564</v>
       </c>
       <c r="X107" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y107" s="4">
         <v>0.7</v>
@@ -11164,7 +11164,7 @@
         <v>564</v>
       </c>
       <c r="X108" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y108" s="4">
         <v>0.7</v>
@@ -11241,7 +11241,7 @@
         <v>564</v>
       </c>
       <c r="X109" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y109" s="4">
         <v>0.7</v>
@@ -11318,7 +11318,7 @@
         <v>564</v>
       </c>
       <c r="X110" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y110" s="4">
         <v>0.7</v>
@@ -11395,7 +11395,7 @@
         <v>564</v>
       </c>
       <c r="X111" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y111" s="4">
         <v>0.7</v>
@@ -11472,7 +11472,7 @@
         <v>564</v>
       </c>
       <c r="X112" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y112" s="4">
         <v>0.7</v>
@@ -11549,7 +11549,7 @@
         <v>564</v>
       </c>
       <c r="X113" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y113" s="4">
         <v>0.7</v>
@@ -11626,7 +11626,7 @@
         <v>564</v>
       </c>
       <c r="X114" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y114" s="4">
         <v>0.7</v>
@@ -11703,7 +11703,7 @@
         <v>564</v>
       </c>
       <c r="X115" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y115" s="4">
         <v>0.7</v>
@@ -11780,7 +11780,7 @@
         <v>564</v>
       </c>
       <c r="X116" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y116" s="4">
         <v>0.7</v>
@@ -11857,7 +11857,7 @@
         <v>564</v>
       </c>
       <c r="X117" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y117" s="4">
         <v>0.7</v>
@@ -11934,7 +11934,7 @@
         <v>564</v>
       </c>
       <c r="X118" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y118" s="4">
         <v>0.7</v>
@@ -12011,7 +12011,7 @@
         <v>564</v>
       </c>
       <c r="X119" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y119" s="4">
         <v>0.7</v>
@@ -12088,7 +12088,7 @@
         <v>564</v>
       </c>
       <c r="X120" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y120" s="4">
         <v>0.7</v>
@@ -12165,7 +12165,7 @@
         <v>564</v>
       </c>
       <c r="X121" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y121" s="4">
         <v>0.7</v>
@@ -12242,7 +12242,7 @@
         <v>564</v>
       </c>
       <c r="X122" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y122" s="4">
         <v>0.7</v>
@@ -12319,7 +12319,7 @@
         <v>564</v>
       </c>
       <c r="X123" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y123" s="4">
         <v>0.7</v>
@@ -12396,7 +12396,7 @@
         <v>564</v>
       </c>
       <c r="X124" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y124" s="4">
         <v>0.7</v>
@@ -12473,7 +12473,7 @@
         <v>564</v>
       </c>
       <c r="X125" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y125" s="4">
         <v>0.7</v>
@@ -12550,7 +12550,7 @@
         <v>564</v>
       </c>
       <c r="X126" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y126" s="4">
         <v>0.7</v>
@@ -12627,7 +12627,7 @@
         <v>564</v>
       </c>
       <c r="X127" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y127" s="4">
         <v>0.7</v>
@@ -12704,7 +12704,7 @@
         <v>564</v>
       </c>
       <c r="X128" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y128" s="4">
         <v>0.7</v>
@@ -12781,7 +12781,7 @@
         <v>564</v>
       </c>
       <c r="X129" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y129" s="4">
         <v>0.7</v>
@@ -12858,7 +12858,7 @@
         <v>564</v>
       </c>
       <c r="X130" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y130" s="4">
         <v>0.7</v>
@@ -12935,7 +12935,7 @@
         <v>564</v>
       </c>
       <c r="X131" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y131" s="4">
         <v>0.7</v>
@@ -13012,7 +13012,7 @@
         <v>564</v>
       </c>
       <c r="X132" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y132" s="4">
         <v>0.7</v>
@@ -13089,7 +13089,7 @@
         <v>564</v>
       </c>
       <c r="X133" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y133" s="4">
         <v>0.7</v>
@@ -13166,7 +13166,7 @@
         <v>564</v>
       </c>
       <c r="X134" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y134" s="4">
         <v>0.7</v>
@@ -13243,7 +13243,7 @@
         <v>564</v>
       </c>
       <c r="X135" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y135" s="4">
         <v>0.7</v>
@@ -13320,7 +13320,7 @@
         <v>564</v>
       </c>
       <c r="X136" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y136" s="4">
         <v>0.7</v>
@@ -13397,7 +13397,7 @@
         <v>564</v>
       </c>
       <c r="X137" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y137" s="4">
         <v>0.7</v>
@@ -13474,7 +13474,7 @@
         <v>564</v>
       </c>
       <c r="X138" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y138" s="4">
         <v>0.7</v>
@@ -13551,7 +13551,7 @@
         <v>564</v>
       </c>
       <c r="X139" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y139" s="4">
         <v>0.7</v>
@@ -13628,7 +13628,7 @@
         <v>564</v>
       </c>
       <c r="X140" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y140" s="4">
         <v>0.7</v>
@@ -13705,7 +13705,7 @@
         <v>564</v>
       </c>
       <c r="X141" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y141" s="4">
         <v>0.7</v>
@@ -13782,7 +13782,7 @@
         <v>564</v>
       </c>
       <c r="X142" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y142" s="4">
         <v>0.7</v>
@@ -13859,7 +13859,7 @@
         <v>564</v>
       </c>
       <c r="X143" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y143" s="4">
         <v>0.7</v>
@@ -13936,7 +13936,7 @@
         <v>564</v>
       </c>
       <c r="X144" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y144" s="4">
         <v>0.7</v>
@@ -14013,7 +14013,7 @@
         <v>564</v>
       </c>
       <c r="X145" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y145" s="4">
         <v>0.7</v>
@@ -14090,7 +14090,7 @@
         <v>564</v>
       </c>
       <c r="X146" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y146" s="4">
         <v>0.7</v>
@@ -14167,7 +14167,7 @@
         <v>564</v>
       </c>
       <c r="X147" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y147" s="4">
         <v>0.7</v>
@@ -14244,7 +14244,7 @@
         <v>564</v>
       </c>
       <c r="X148" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y148" s="4">
         <v>0.7</v>
@@ -14321,7 +14321,7 @@
         <v>564</v>
       </c>
       <c r="X149" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y149" s="4">
         <v>0.7</v>
@@ -14398,7 +14398,7 @@
         <v>564</v>
       </c>
       <c r="X150" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y150" s="4">
         <v>0.7</v>
@@ -14475,7 +14475,7 @@
         <v>564</v>
       </c>
       <c r="X151" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y151" s="4">
         <v>0.7</v>
@@ -14552,7 +14552,7 @@
         <v>564</v>
       </c>
       <c r="X152" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y152" s="4">
         <v>0.7</v>
@@ -14629,7 +14629,7 @@
         <v>564</v>
       </c>
       <c r="X153" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y153" s="4">
         <v>0.7</v>
@@ -14706,7 +14706,7 @@
         <v>564</v>
       </c>
       <c r="X154" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y154" s="4">
         <v>0.7</v>
@@ -14783,7 +14783,7 @@
         <v>564</v>
       </c>
       <c r="X155" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y155" s="4">
         <v>0.7</v>
@@ -14860,7 +14860,7 @@
         <v>564</v>
       </c>
       <c r="X156" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y156" s="4">
         <v>0.7</v>
@@ -14937,7 +14937,7 @@
         <v>564</v>
       </c>
       <c r="X157" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y157" s="4">
         <v>0.7</v>
@@ -15014,7 +15014,7 @@
         <v>564</v>
       </c>
       <c r="X158" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y158" s="4">
         <v>0.7</v>
@@ -15091,7 +15091,7 @@
         <v>564</v>
       </c>
       <c r="X159" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y159" s="4">
         <v>0.7</v>
@@ -15168,7 +15168,7 @@
         <v>564</v>
       </c>
       <c r="X160" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y160" s="4">
         <v>0.7</v>
@@ -15245,7 +15245,7 @@
         <v>564</v>
       </c>
       <c r="X161" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y161" s="4">
         <v>0.7</v>
@@ -15322,7 +15322,7 @@
         <v>564</v>
       </c>
       <c r="X162" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y162" s="4">
         <v>0.7</v>
@@ -15399,7 +15399,7 @@
         <v>564</v>
       </c>
       <c r="X163" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y163" s="4">
         <v>0.7</v>
@@ -15476,7 +15476,7 @@
         <v>564</v>
       </c>
       <c r="X164" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y164" s="4">
         <v>0.7</v>
@@ -15553,7 +15553,7 @@
         <v>564</v>
       </c>
       <c r="X165" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y165" s="4">
         <v>0.7</v>
@@ -15630,7 +15630,7 @@
         <v>564</v>
       </c>
       <c r="X166" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y166" s="4">
         <v>0.7</v>
@@ -15707,7 +15707,7 @@
         <v>564</v>
       </c>
       <c r="X167" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y167" s="4">
         <v>0.7</v>
@@ -15784,7 +15784,7 @@
         <v>564</v>
       </c>
       <c r="X168" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y168" s="4">
         <v>0.7</v>
@@ -15861,7 +15861,7 @@
         <v>564</v>
       </c>
       <c r="X169" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y169" s="4">
         <v>0.7</v>
@@ -15938,7 +15938,7 @@
         <v>564</v>
       </c>
       <c r="X170" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y170" s="4">
         <v>0.7</v>
@@ -16015,7 +16015,7 @@
         <v>564</v>
       </c>
       <c r="X171" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y171" s="4">
         <v>0.7</v>
@@ -16092,7 +16092,7 @@
         <v>564</v>
       </c>
       <c r="X172" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y172" s="4">
         <v>0.7</v>
@@ -16169,7 +16169,7 @@
         <v>564</v>
       </c>
       <c r="X173" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y173" s="4">
         <v>0.7</v>
@@ -16246,7 +16246,7 @@
         <v>564</v>
       </c>
       <c r="X174" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y174" s="4">
         <v>0.7</v>
@@ -16323,7 +16323,7 @@
         <v>564</v>
       </c>
       <c r="X175" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y175" s="4">
         <v>0.7</v>
@@ -16400,7 +16400,7 @@
         <v>564</v>
       </c>
       <c r="X176" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y176" s="4">
         <v>0.7</v>
@@ -16477,7 +16477,7 @@
         <v>564</v>
       </c>
       <c r="X177" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y177" s="4">
         <v>0.7</v>
@@ -16554,7 +16554,7 @@
         <v>564</v>
       </c>
       <c r="X178" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y178" s="4">
         <v>0.7</v>
@@ -16631,7 +16631,7 @@
         <v>564</v>
       </c>
       <c r="X179" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y179" s="4">
         <v>0.7</v>
@@ -16708,7 +16708,7 @@
         <v>564</v>
       </c>
       <c r="X180" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y180" s="4">
         <v>0.7</v>
@@ -16785,7 +16785,7 @@
         <v>564</v>
       </c>
       <c r="X181" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y181" s="4">
         <v>0.7</v>
@@ -16862,7 +16862,7 @@
         <v>564</v>
       </c>
       <c r="X182" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y182" s="4">
         <v>0.7</v>
@@ -16939,7 +16939,7 @@
         <v>564</v>
       </c>
       <c r="X183" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y183" s="4">
         <v>0.7</v>
@@ -17016,7 +17016,7 @@
         <v>564</v>
       </c>
       <c r="X184" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y184" s="4">
         <v>0.7</v>
@@ -17093,7 +17093,7 @@
         <v>564</v>
       </c>
       <c r="X185" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y185" s="4">
         <v>0.7</v>
@@ -17170,7 +17170,7 @@
         <v>564</v>
       </c>
       <c r="X186" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y186" s="4">
         <v>0.7</v>
@@ -17247,7 +17247,7 @@
         <v>564</v>
       </c>
       <c r="X187" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y187" s="4">
         <v>0.7</v>
@@ -17324,7 +17324,7 @@
         <v>564</v>
       </c>
       <c r="X188" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y188" s="4">
         <v>0.7</v>
@@ -17401,7 +17401,7 @@
         <v>564</v>
       </c>
       <c r="X189" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y189" s="4">
         <v>0.7</v>
@@ -17478,7 +17478,7 @@
         <v>564</v>
       </c>
       <c r="X190" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y190" s="4">
         <v>0.7</v>
@@ -17555,7 +17555,7 @@
         <v>564</v>
       </c>
       <c r="X191" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y191" s="4">
         <v>0.7</v>
@@ -17632,7 +17632,7 @@
         <v>564</v>
       </c>
       <c r="X192" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y192" s="4">
         <v>0.7</v>
@@ -17709,7 +17709,7 @@
         <v>564</v>
       </c>
       <c r="X193" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y193" s="4">
         <v>0.7</v>
@@ -17786,7 +17786,7 @@
         <v>564</v>
       </c>
       <c r="X194" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y194" s="4">
         <v>0.7</v>
@@ -17863,7 +17863,7 @@
         <v>564</v>
       </c>
       <c r="X195" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y195" s="4">
         <v>0.7</v>
@@ -17940,7 +17940,7 @@
         <v>564</v>
       </c>
       <c r="X196" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y196" s="4">
         <v>0.7</v>
@@ -18017,7 +18017,7 @@
         <v>564</v>
       </c>
       <c r="X197" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y197" s="4">
         <v>0.7</v>
@@ -18094,7 +18094,7 @@
         <v>564</v>
       </c>
       <c r="X198" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y198" s="4">
         <v>0.7</v>
@@ -18171,7 +18171,7 @@
         <v>564</v>
       </c>
       <c r="X199" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y199" s="4">
         <v>0.7</v>
@@ -18248,7 +18248,7 @@
         <v>564</v>
       </c>
       <c r="X200" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y200" s="4">
         <v>0.7</v>
@@ -18325,7 +18325,7 @@
         <v>564</v>
       </c>
       <c r="X201" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y201" s="4">
         <v>0.7</v>
@@ -18402,7 +18402,7 @@
         <v>564</v>
       </c>
       <c r="X202" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y202" s="4">
         <v>0.7</v>
@@ -18479,7 +18479,7 @@
         <v>564</v>
       </c>
       <c r="X203" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y203" s="4">
         <v>0.7</v>
@@ -18556,7 +18556,7 @@
         <v>564</v>
       </c>
       <c r="X204" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y204" s="4">
         <v>0.7</v>
@@ -18633,7 +18633,7 @@
         <v>564</v>
       </c>
       <c r="X205" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y205" s="4">
         <v>0.7</v>
@@ -18710,7 +18710,7 @@
         <v>564</v>
       </c>
       <c r="X206" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y206" s="4">
         <v>0.7</v>
@@ -18787,7 +18787,7 @@
         <v>564</v>
       </c>
       <c r="X207" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y207" s="4">
         <v>0.7</v>
@@ -18864,7 +18864,7 @@
         <v>564</v>
       </c>
       <c r="X208" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y208" s="4">
         <v>0.7</v>
@@ -18941,7 +18941,7 @@
         <v>564</v>
       </c>
       <c r="X209" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y209" s="4">
         <v>0.7</v>
@@ -19018,7 +19018,7 @@
         <v>564</v>
       </c>
       <c r="X210" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y210" s="4">
         <v>0.7</v>
@@ -19095,7 +19095,7 @@
         <v>564</v>
       </c>
       <c r="X211" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y211" s="4">
         <v>0.7</v>
@@ -19172,7 +19172,7 @@
         <v>564</v>
       </c>
       <c r="X212" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y212" s="4">
         <v>0.7</v>
@@ -19249,7 +19249,7 @@
         <v>564</v>
       </c>
       <c r="X213" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y213" s="4">
         <v>0.7</v>
@@ -19326,7 +19326,7 @@
         <v>564</v>
       </c>
       <c r="X214" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y214" s="4">
         <v>0.7</v>
@@ -19403,7 +19403,7 @@
         <v>564</v>
       </c>
       <c r="X215" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y215" s="4">
         <v>0.7</v>
@@ -19480,7 +19480,7 @@
         <v>564</v>
       </c>
       <c r="X216" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y216" s="4">
         <v>0.7</v>
@@ -19557,7 +19557,7 @@
         <v>564</v>
       </c>
       <c r="X217" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y217" s="4">
         <v>0.7</v>
@@ -19634,7 +19634,7 @@
         <v>564</v>
       </c>
       <c r="X218" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y218" s="4">
         <v>0.7</v>
@@ -19711,7 +19711,7 @@
         <v>564</v>
       </c>
       <c r="X219" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y219" s="4">
         <v>0.7</v>
@@ -19788,7 +19788,7 @@
         <v>564</v>
       </c>
       <c r="X220" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y220" s="4">
         <v>0.7</v>
@@ -19865,7 +19865,7 @@
         <v>564</v>
       </c>
       <c r="X221" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y221" s="4">
         <v>0.7</v>
@@ -19942,7 +19942,7 @@
         <v>564</v>
       </c>
       <c r="X222" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y222" s="4">
         <v>0.7</v>
@@ -20019,7 +20019,7 @@
         <v>564</v>
       </c>
       <c r="X223" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y223" s="4">
         <v>0.7</v>
@@ -20096,7 +20096,7 @@
         <v>564</v>
       </c>
       <c r="X224" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y224" s="4">
         <v>0.7</v>
@@ -20173,7 +20173,7 @@
         <v>564</v>
       </c>
       <c r="X225" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y225" s="4">
         <v>0.7</v>
@@ -20250,7 +20250,7 @@
         <v>564</v>
       </c>
       <c r="X226" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y226" s="4">
         <v>0.7</v>
@@ -20327,7 +20327,7 @@
         <v>564</v>
       </c>
       <c r="X227" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y227" s="4">
         <v>0.7</v>
@@ -20404,7 +20404,7 @@
         <v>564</v>
       </c>
       <c r="X228" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y228" s="4">
         <v>0.7</v>
@@ -20481,7 +20481,7 @@
         <v>564</v>
       </c>
       <c r="X229" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y229" s="4">
         <v>0.7</v>
@@ -20558,7 +20558,7 @@
         <v>564</v>
       </c>
       <c r="X230" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y230" s="4">
         <v>0.7</v>
@@ -20635,7 +20635,7 @@
         <v>564</v>
       </c>
       <c r="X231" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y231" s="4">
         <v>0.7</v>
@@ -20712,7 +20712,7 @@
         <v>564</v>
       </c>
       <c r="X232" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y232" s="4">
         <v>0.7</v>
@@ -20789,7 +20789,7 @@
         <v>564</v>
       </c>
       <c r="X233" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y233" s="4">
         <v>0.7</v>
@@ -20866,7 +20866,7 @@
         <v>564</v>
       </c>
       <c r="X234" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y234" s="4">
         <v>0.7</v>
@@ -20943,7 +20943,7 @@
         <v>564</v>
       </c>
       <c r="X235" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y235" s="4">
         <v>0.7</v>
@@ -21020,7 +21020,7 @@
         <v>564</v>
       </c>
       <c r="X236" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y236" s="4">
         <v>0.7</v>
@@ -21097,7 +21097,7 @@
         <v>564</v>
       </c>
       <c r="X237" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y237" s="4">
         <v>0.7</v>
@@ -21174,7 +21174,7 @@
         <v>564</v>
       </c>
       <c r="X238" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y238" s="4">
         <v>0.7</v>
@@ -21251,7 +21251,7 @@
         <v>564</v>
       </c>
       <c r="X239" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y239" s="4">
         <v>0.7</v>
@@ -21328,7 +21328,7 @@
         <v>564</v>
       </c>
       <c r="X240" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y240" s="4">
         <v>0.7</v>
@@ -21405,7 +21405,7 @@
         <v>564</v>
       </c>
       <c r="X241" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y241" s="4">
         <v>0.7</v>
@@ -21482,7 +21482,7 @@
         <v>564</v>
       </c>
       <c r="X242" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y242" s="4">
         <v>0.7</v>
@@ -21559,7 +21559,7 @@
         <v>564</v>
       </c>
       <c r="X243" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y243" s="4">
         <v>0.7</v>
@@ -21636,7 +21636,7 @@
         <v>564</v>
       </c>
       <c r="X244" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y244" s="4">
         <v>0.7</v>
@@ -21713,7 +21713,7 @@
         <v>564</v>
       </c>
       <c r="X245" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y245" s="4">
         <v>0.7</v>
@@ -21790,7 +21790,7 @@
         <v>564</v>
       </c>
       <c r="X246" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y246" s="4">
         <v>0.7</v>
@@ -21867,7 +21867,7 @@
         <v>564</v>
       </c>
       <c r="X247" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y247" s="4">
         <v>0.7</v>
@@ -21944,7 +21944,7 @@
         <v>564</v>
       </c>
       <c r="X248" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y248" s="4">
         <v>0.7</v>
@@ -22021,7 +22021,7 @@
         <v>564</v>
       </c>
       <c r="X249" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y249" s="4">
         <v>0.7</v>
@@ -22098,7 +22098,7 @@
         <v>564</v>
       </c>
       <c r="X250" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y250" s="4">
         <v>0.7</v>
@@ -22175,7 +22175,7 @@
         <v>564</v>
       </c>
       <c r="X251" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y251" s="4">
         <v>0.7</v>
@@ -22252,7 +22252,7 @@
         <v>564</v>
       </c>
       <c r="X252" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y252" s="4">
         <v>0.7</v>
@@ -22329,7 +22329,7 @@
         <v>564</v>
       </c>
       <c r="X253" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y253" s="4">
         <v>0.7</v>
@@ -22406,7 +22406,7 @@
         <v>564</v>
       </c>
       <c r="X254" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y254" s="4">
         <v>0.7</v>
@@ -22483,7 +22483,7 @@
         <v>564</v>
       </c>
       <c r="X255" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y255" s="4">
         <v>0.7</v>
@@ -22560,7 +22560,7 @@
         <v>564</v>
       </c>
       <c r="X256" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y256" s="4">
         <v>0.7</v>
@@ -22637,7 +22637,7 @@
         <v>564</v>
       </c>
       <c r="X257" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y257" s="4">
         <v>0.7</v>
@@ -22714,7 +22714,7 @@
         <v>564</v>
       </c>
       <c r="X258" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y258" s="4">
         <v>0.7</v>
@@ -22791,7 +22791,7 @@
         <v>564</v>
       </c>
       <c r="X259" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y259" s="4">
         <v>0.7</v>
@@ -22868,7 +22868,7 @@
         <v>564</v>
       </c>
       <c r="X260" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y260" s="4">
         <v>0.7</v>
@@ -22945,7 +22945,7 @@
         <v>564</v>
       </c>
       <c r="X261" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y261" s="4">
         <v>0.7</v>
@@ -23022,7 +23022,7 @@
         <v>564</v>
       </c>
       <c r="X262" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y262" s="4">
         <v>0.7</v>
@@ -23099,7 +23099,7 @@
         <v>564</v>
       </c>
       <c r="X263" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y263" s="4">
         <v>0.7</v>
@@ -23176,7 +23176,7 @@
         <v>564</v>
       </c>
       <c r="X264" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y264" s="4">
         <v>0.7</v>
@@ -23253,7 +23253,7 @@
         <v>564</v>
       </c>
       <c r="X265" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y265" s="4">
         <v>0.7</v>
@@ -23330,7 +23330,7 @@
         <v>564</v>
       </c>
       <c r="X266" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y266" s="4">
         <v>0.7</v>
@@ -23407,7 +23407,7 @@
         <v>564</v>
       </c>
       <c r="X267" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y267" s="4">
         <v>0.7</v>
@@ -23484,7 +23484,7 @@
         <v>564</v>
       </c>
       <c r="X268" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y268" s="4">
         <v>0.7</v>
@@ -23561,7 +23561,7 @@
         <v>564</v>
       </c>
       <c r="X269" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y269" s="4">
         <v>0.7</v>
@@ -23638,7 +23638,7 @@
         <v>564</v>
       </c>
       <c r="X270" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y270" s="4">
         <v>0.7</v>
@@ -23715,7 +23715,7 @@
         <v>564</v>
       </c>
       <c r="X271" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y271" s="4">
         <v>0.7</v>
@@ -23792,7 +23792,7 @@
         <v>564</v>
       </c>
       <c r="X272" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y272" s="4">
         <v>0.7</v>
@@ -23869,7 +23869,7 @@
         <v>564</v>
       </c>
       <c r="X273" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y273" s="4">
         <v>0.7</v>
@@ -23946,7 +23946,7 @@
         <v>564</v>
       </c>
       <c r="X274" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y274" s="4">
         <v>0.7</v>
@@ -24023,7 +24023,7 @@
         <v>564</v>
       </c>
       <c r="X275" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y275" s="4">
         <v>0.7</v>
@@ -24100,7 +24100,7 @@
         <v>564</v>
       </c>
       <c r="X276" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y276" s="4">
         <v>0.7</v>
@@ -24177,7 +24177,7 @@
         <v>564</v>
       </c>
       <c r="X277" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y277" s="4">
         <v>0.7</v>
@@ -24254,7 +24254,7 @@
         <v>564</v>
       </c>
       <c r="X278" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y278" s="4">
         <v>0.7</v>
@@ -24331,7 +24331,7 @@
         <v>564</v>
       </c>
       <c r="X279" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y279" s="4">
         <v>0.7</v>
@@ -24408,7 +24408,7 @@
         <v>564</v>
       </c>
       <c r="X280" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y280" s="4">
         <v>0.7</v>
@@ -24485,7 +24485,7 @@
         <v>564</v>
       </c>
       <c r="X281" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y281" s="4">
         <v>0.7</v>
@@ -24562,7 +24562,7 @@
         <v>564</v>
       </c>
       <c r="X282" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y282" s="4">
         <v>0.7</v>
@@ -24639,7 +24639,7 @@
         <v>564</v>
       </c>
       <c r="X283" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y283" s="4">
         <v>0.7</v>
@@ -24716,7 +24716,7 @@
         <v>564</v>
       </c>
       <c r="X284" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y284" s="4">
         <v>0.7</v>
@@ -24793,7 +24793,7 @@
         <v>564</v>
       </c>
       <c r="X285" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y285" s="4">
         <v>0.7</v>
@@ -24870,7 +24870,7 @@
         <v>564</v>
       </c>
       <c r="X286" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y286" s="4">
         <v>0.7</v>
@@ -24947,7 +24947,7 @@
         <v>564</v>
       </c>
       <c r="X287" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y287" s="4">
         <v>0.7</v>
@@ -25024,7 +25024,7 @@
         <v>564</v>
       </c>
       <c r="X288" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y288" s="4">
         <v>0.7</v>
@@ -25101,7 +25101,7 @@
         <v>564</v>
       </c>
       <c r="X289" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y289" s="4">
         <v>0.7</v>
@@ -25178,7 +25178,7 @@
         <v>564</v>
       </c>
       <c r="X290" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y290" s="4">
         <v>0.7</v>
@@ -25255,7 +25255,7 @@
         <v>564</v>
       </c>
       <c r="X291" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y291" s="4">
         <v>0.7</v>
@@ -25332,7 +25332,7 @@
         <v>564</v>
       </c>
       <c r="X292" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y292" s="4">
         <v>0.7</v>
@@ -25409,7 +25409,7 @@
         <v>564</v>
       </c>
       <c r="X293" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y293" s="4">
         <v>0.7</v>
@@ -25486,7 +25486,7 @@
         <v>564</v>
       </c>
       <c r="X294" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y294" s="4">
         <v>0.7</v>
@@ -25563,7 +25563,7 @@
         <v>564</v>
       </c>
       <c r="X295" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y295" s="4">
         <v>0.7</v>
@@ -25640,7 +25640,7 @@
         <v>564</v>
       </c>
       <c r="X296" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y296" s="4">
         <v>0.7</v>
@@ -25717,7 +25717,7 @@
         <v>564</v>
       </c>
       <c r="X297" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y297" s="4">
         <v>0.7</v>
@@ -25794,7 +25794,7 @@
         <v>564</v>
       </c>
       <c r="X298" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y298" s="4">
         <v>0.7</v>
@@ -25871,7 +25871,7 @@
         <v>564</v>
       </c>
       <c r="X299" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y299" s="4">
         <v>0.7</v>
@@ -25948,7 +25948,7 @@
         <v>564</v>
       </c>
       <c r="X300" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y300" s="4">
         <v>0.7</v>
@@ -26025,7 +26025,7 @@
         <v>564</v>
       </c>
       <c r="X301" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y301" s="4">
         <v>0.7</v>
@@ -26102,7 +26102,7 @@
         <v>564</v>
       </c>
       <c r="X302" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y302" s="4">
         <v>0.7</v>
@@ -26179,7 +26179,7 @@
         <v>564</v>
       </c>
       <c r="X303" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y303" s="4">
         <v>0.7</v>
@@ -26256,7 +26256,7 @@
         <v>564</v>
       </c>
       <c r="X304" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y304" s="4">
         <v>0.7</v>
@@ -26333,7 +26333,7 @@
         <v>564</v>
       </c>
       <c r="X305" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y305" s="4">
         <v>0.7</v>
@@ -26410,7 +26410,7 @@
         <v>564</v>
       </c>
       <c r="X306" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y306" s="4">
         <v>0.7</v>
@@ -26487,7 +26487,7 @@
         <v>564</v>
       </c>
       <c r="X307" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y307" s="4">
         <v>0.7</v>
@@ -26564,7 +26564,7 @@
         <v>564</v>
       </c>
       <c r="X308" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y308" s="4">
         <v>0.7</v>
@@ -26641,7 +26641,7 @@
         <v>564</v>
       </c>
       <c r="X309" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y309" s="4">
         <v>0.7</v>
@@ -26718,7 +26718,7 @@
         <v>564</v>
       </c>
       <c r="X310" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y310" s="4">
         <v>0.7</v>
@@ -26795,7 +26795,7 @@
         <v>564</v>
       </c>
       <c r="X311" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y311" s="4">
         <v>0.7</v>
@@ -26872,7 +26872,7 @@
         <v>564</v>
       </c>
       <c r="X312" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y312" s="4">
         <v>0.7</v>
@@ -26949,7 +26949,7 @@
         <v>564</v>
       </c>
       <c r="X313" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y313" s="4">
         <v>0.7</v>
@@ -27026,7 +27026,7 @@
         <v>564</v>
       </c>
       <c r="X314" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y314" s="4">
         <v>0.7</v>
@@ -27103,7 +27103,7 @@
         <v>564</v>
       </c>
       <c r="X315" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y315" s="4">
         <v>0.7</v>
@@ -27180,7 +27180,7 @@
         <v>564</v>
       </c>
       <c r="X316" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y316" s="4">
         <v>0.7</v>
@@ -27257,7 +27257,7 @@
         <v>564</v>
       </c>
       <c r="X317" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y317" s="4">
         <v>0.7</v>
@@ -27334,7 +27334,7 @@
         <v>564</v>
       </c>
       <c r="X318" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y318" s="4">
         <v>0.7</v>
@@ -27411,7 +27411,7 @@
         <v>564</v>
       </c>
       <c r="X319" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y319" s="4">
         <v>0.7</v>
@@ -27488,7 +27488,7 @@
         <v>564</v>
       </c>
       <c r="X320" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y320" s="4">
         <v>0.7</v>
@@ -27565,7 +27565,7 @@
         <v>564</v>
       </c>
       <c r="X321" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y321" s="4">
         <v>0.7</v>
@@ -27642,7 +27642,7 @@
         <v>564</v>
       </c>
       <c r="X322" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y322" s="4">
         <v>0.7</v>
@@ -27719,7 +27719,7 @@
         <v>564</v>
       </c>
       <c r="X323" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y323" s="4">
         <v>0.7</v>
@@ -27796,7 +27796,7 @@
         <v>564</v>
       </c>
       <c r="X324" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y324" s="4">
         <v>0.7</v>
@@ -27873,7 +27873,7 @@
         <v>564</v>
       </c>
       <c r="X325" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y325" s="4">
         <v>0.7</v>
@@ -27950,7 +27950,7 @@
         <v>564</v>
       </c>
       <c r="X326" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y326" s="4">
         <v>0.7</v>
@@ -28027,7 +28027,7 @@
         <v>564</v>
       </c>
       <c r="X327" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y327" s="4">
         <v>0.7</v>
@@ -28104,7 +28104,7 @@
         <v>564</v>
       </c>
       <c r="X328" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y328" s="4">
         <v>0.7</v>
@@ -28181,7 +28181,7 @@
         <v>564</v>
       </c>
       <c r="X329" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y329" s="4">
         <v>0.7</v>
@@ -28258,7 +28258,7 @@
         <v>564</v>
       </c>
       <c r="X330" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y330" s="4">
         <v>0.7</v>
@@ -28335,7 +28335,7 @@
         <v>564</v>
       </c>
       <c r="X331" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y331" s="4">
         <v>0.7</v>
@@ -28412,7 +28412,7 @@
         <v>564</v>
       </c>
       <c r="X332" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y332" s="4">
         <v>0.7</v>
@@ -28489,7 +28489,7 @@
         <v>564</v>
       </c>
       <c r="X333" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y333" s="4">
         <v>0.7</v>
@@ -28566,7 +28566,7 @@
         <v>564</v>
       </c>
       <c r="X334" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y334" s="4">
         <v>0.7</v>
@@ -28643,7 +28643,7 @@
         <v>564</v>
       </c>
       <c r="X335" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y335" s="4">
         <v>0.7</v>
@@ -28720,7 +28720,7 @@
         <v>564</v>
       </c>
       <c r="X336" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y336" s="4">
         <v>0.7</v>
@@ -28797,7 +28797,7 @@
         <v>564</v>
       </c>
       <c r="X337" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y337" s="4">
         <v>0.7</v>
@@ -28874,7 +28874,7 @@
         <v>564</v>
       </c>
       <c r="X338" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y338" s="4">
         <v>0.7</v>
@@ -28951,7 +28951,7 @@
         <v>564</v>
       </c>
       <c r="X339" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y339" s="4">
         <v>0.7</v>
@@ -29028,7 +29028,7 @@
         <v>564</v>
       </c>
       <c r="X340" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y340" s="4">
         <v>0.7</v>
@@ -29105,7 +29105,7 @@
         <v>564</v>
       </c>
       <c r="X341" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y341" s="4">
         <v>0.7</v>
@@ -29182,7 +29182,7 @@
         <v>564</v>
       </c>
       <c r="X342" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y342" s="4">
         <v>0.7</v>
@@ -29259,7 +29259,7 @@
         <v>564</v>
       </c>
       <c r="X343" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y343" s="4">
         <v>0.7</v>
@@ -29336,7 +29336,7 @@
         <v>564</v>
       </c>
       <c r="X344" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y344" s="4">
         <v>0.7</v>
@@ -29413,7 +29413,7 @@
         <v>564</v>
       </c>
       <c r="X345" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y345" s="4">
         <v>0.7</v>
@@ -29490,7 +29490,7 @@
         <v>564</v>
       </c>
       <c r="X346" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y346" s="4">
         <v>0.7</v>
@@ -29567,7 +29567,7 @@
         <v>564</v>
       </c>
       <c r="X347" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y347" s="4">
         <v>0.7</v>
@@ -29644,7 +29644,7 @@
         <v>564</v>
       </c>
       <c r="X348" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y348" s="4">
         <v>0.7</v>
@@ -29721,7 +29721,7 @@
         <v>564</v>
       </c>
       <c r="X349" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y349" s="4">
         <v>0.7</v>
@@ -29798,7 +29798,7 @@
         <v>564</v>
       </c>
       <c r="X350" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y350" s="4">
         <v>0.7</v>
@@ -29875,7 +29875,7 @@
         <v>564</v>
       </c>
       <c r="X351" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y351" s="4">
         <v>0.7</v>
@@ -29952,7 +29952,7 @@
         <v>564</v>
       </c>
       <c r="X352" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y352" s="4">
         <v>0.7</v>
@@ -30029,7 +30029,7 @@
         <v>564</v>
       </c>
       <c r="X353" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y353" s="4">
         <v>0.7</v>
@@ -30106,7 +30106,7 @@
         <v>564</v>
       </c>
       <c r="X354" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y354" s="4">
         <v>0.7</v>
@@ -30183,7 +30183,7 @@
         <v>564</v>
       </c>
       <c r="X355" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y355" s="4">
         <v>0.7</v>
@@ -30260,7 +30260,7 @@
         <v>564</v>
       </c>
       <c r="X356" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y356" s="4">
         <v>0.7</v>
@@ -30337,7 +30337,7 @@
         <v>564</v>
       </c>
       <c r="X357" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y357" s="4">
         <v>0.7</v>
@@ -30414,7 +30414,7 @@
         <v>564</v>
       </c>
       <c r="X358" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y358" s="4">
         <v>0.7</v>
@@ -30491,7 +30491,7 @@
         <v>564</v>
       </c>
       <c r="X359" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y359" s="4">
         <v>0.7</v>
@@ -30568,7 +30568,7 @@
         <v>564</v>
       </c>
       <c r="X360" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y360" s="4">
         <v>0.7</v>
@@ -30645,7 +30645,7 @@
         <v>564</v>
       </c>
       <c r="X361" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y361" s="4">
         <v>0.7</v>
@@ -30722,7 +30722,7 @@
         <v>564</v>
       </c>
       <c r="X362" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y362" s="4">
         <v>0.7</v>
@@ -30799,7 +30799,7 @@
         <v>564</v>
       </c>
       <c r="X363" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y363" s="4">
         <v>0.7</v>
@@ -30876,7 +30876,7 @@
         <v>564</v>
       </c>
       <c r="X364" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y364" s="4">
         <v>0.7</v>
@@ -30953,7 +30953,7 @@
         <v>564</v>
       </c>
       <c r="X365" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y365" s="4">
         <v>0.7</v>
@@ -31030,7 +31030,7 @@
         <v>564</v>
       </c>
       <c r="X366" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y366" s="4">
         <v>0.7</v>
@@ -31107,7 +31107,7 @@
         <v>564</v>
       </c>
       <c r="X367" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y367" s="4">
         <v>0.7</v>
@@ -31184,7 +31184,7 @@
         <v>564</v>
       </c>
       <c r="X368" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y368" s="4">
         <v>0.7</v>
@@ -31261,7 +31261,7 @@
         <v>564</v>
       </c>
       <c r="X369" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y369" s="4">
         <v>0.7</v>
@@ -31338,7 +31338,7 @@
         <v>564</v>
       </c>
       <c r="X370" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y370" s="4">
         <v>0.7</v>
@@ -31415,7 +31415,7 @@
         <v>564</v>
       </c>
       <c r="X371" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y371" s="4">
         <v>0.7</v>
@@ -31492,7 +31492,7 @@
         <v>564</v>
       </c>
       <c r="X372" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y372" s="4">
         <v>0.7</v>
@@ -31569,7 +31569,7 @@
         <v>564</v>
       </c>
       <c r="X373" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y373" s="4">
         <v>0.7</v>
@@ -31646,7 +31646,7 @@
         <v>564</v>
       </c>
       <c r="X374" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y374" s="4">
         <v>0.7</v>
@@ -31723,7 +31723,7 @@
         <v>564</v>
       </c>
       <c r="X375" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y375" s="4">
         <v>0.7</v>
@@ -31800,7 +31800,7 @@
         <v>564</v>
       </c>
       <c r="X376" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y376" s="4">
         <v>0.7</v>
@@ -31877,7 +31877,7 @@
         <v>564</v>
       </c>
       <c r="X377" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y377" s="4">
         <v>0.7</v>
@@ -31954,7 +31954,7 @@
         <v>564</v>
       </c>
       <c r="X378" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y378" s="4">
         <v>0.7</v>
@@ -32031,7 +32031,7 @@
         <v>564</v>
       </c>
       <c r="X379" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y379" s="4">
         <v>0.7</v>
@@ -32108,7 +32108,7 @@
         <v>564</v>
       </c>
       <c r="X380" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y380" s="4">
         <v>0.7</v>
@@ -32185,7 +32185,7 @@
         <v>564</v>
       </c>
       <c r="X381" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y381" s="4">
         <v>0.7</v>
@@ -32262,7 +32262,7 @@
         <v>564</v>
       </c>
       <c r="X382" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y382" s="4">
         <v>0.7</v>
@@ -32339,7 +32339,7 @@
         <v>564</v>
       </c>
       <c r="X383" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y383" s="4">
         <v>0.7</v>
@@ -32416,7 +32416,7 @@
         <v>564</v>
       </c>
       <c r="X384" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y384" s="4">
         <v>0.7</v>
@@ -32493,7 +32493,7 @@
         <v>564</v>
       </c>
       <c r="X385" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y385" s="4">
         <v>0.7</v>
@@ -32570,7 +32570,7 @@
         <v>564</v>
       </c>
       <c r="X386" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y386" s="4">
         <v>0.7</v>
@@ -32647,7 +32647,7 @@
         <v>564</v>
       </c>
       <c r="X387" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y387" s="4">
         <v>0.7</v>
@@ -32724,7 +32724,7 @@
         <v>564</v>
       </c>
       <c r="X388" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y388" s="4">
         <v>0.7</v>
@@ -32801,7 +32801,7 @@
         <v>564</v>
       </c>
       <c r="X389" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y389" s="4">
         <v>0.7</v>
@@ -32878,7 +32878,7 @@
         <v>564</v>
       </c>
       <c r="X390" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y390" s="4">
         <v>0.7</v>
@@ -32955,7 +32955,7 @@
         <v>564</v>
       </c>
       <c r="X391" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y391" s="4">
         <v>0.7</v>
@@ -33032,7 +33032,7 @@
         <v>564</v>
       </c>
       <c r="X392" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y392" s="4">
         <v>0.7</v>
@@ -33109,7 +33109,7 @@
         <v>564</v>
       </c>
       <c r="X393" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y393" s="4">
         <v>0.7</v>
@@ -33186,7 +33186,7 @@
         <v>564</v>
       </c>
       <c r="X394" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y394" s="4">
         <v>0.7</v>
@@ -33263,7 +33263,7 @@
         <v>564</v>
       </c>
       <c r="X395" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y395" s="4">
         <v>0.7</v>
@@ -33340,7 +33340,7 @@
         <v>564</v>
       </c>
       <c r="X396" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y396" s="4">
         <v>0.7</v>
@@ -33417,7 +33417,7 @@
         <v>564</v>
       </c>
       <c r="X397" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y397" s="4">
         <v>0.7</v>
@@ -33494,7 +33494,7 @@
         <v>564</v>
       </c>
       <c r="X398" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y398" s="4">
         <v>0.7</v>
@@ -33571,7 +33571,7 @@
         <v>564</v>
       </c>
       <c r="X399" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y399" s="4">
         <v>0.7</v>
@@ -33648,7 +33648,7 @@
         <v>564</v>
       </c>
       <c r="X400" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y400" s="4">
         <v>0.7</v>
@@ -33725,7 +33725,7 @@
         <v>564</v>
       </c>
       <c r="X401" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y401" s="4">
         <v>0.7</v>
@@ -33802,7 +33802,7 @@
         <v>564</v>
       </c>
       <c r="X402" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y402" s="4">
         <v>0.7</v>
@@ -33879,7 +33879,7 @@
         <v>564</v>
       </c>
       <c r="X403" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y403" s="4">
         <v>0.7</v>
@@ -33956,7 +33956,7 @@
         <v>564</v>
       </c>
       <c r="X404" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y404" s="4">
         <v>0.7</v>
@@ -34033,7 +34033,7 @@
         <v>564</v>
       </c>
       <c r="X405" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y405" s="4">
         <v>0.7</v>
@@ -34110,7 +34110,7 @@
         <v>564</v>
       </c>
       <c r="X406" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y406" s="4">
         <v>0.7</v>
@@ -34187,7 +34187,7 @@
         <v>564</v>
       </c>
       <c r="X407" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y407" s="4">
         <v>0.7</v>
@@ -34264,7 +34264,7 @@
         <v>564</v>
       </c>
       <c r="X408" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y408" s="4">
         <v>0.7</v>
@@ -34341,7 +34341,7 @@
         <v>564</v>
       </c>
       <c r="X409" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y409" s="4">
         <v>0.7</v>
@@ -34418,7 +34418,7 @@
         <v>564</v>
       </c>
       <c r="X410" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y410" s="4">
         <v>0.7</v>
@@ -34495,7 +34495,7 @@
         <v>564</v>
       </c>
       <c r="X411" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y411" s="4">
         <v>0.7</v>
@@ -34572,7 +34572,7 @@
         <v>564</v>
       </c>
       <c r="X412" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y412" s="4">
         <v>0.7</v>
@@ -34649,7 +34649,7 @@
         <v>564</v>
       </c>
       <c r="X413" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y413" s="4">
         <v>0.7</v>
@@ -34726,7 +34726,7 @@
         <v>564</v>
       </c>
       <c r="X414" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y414" s="4">
         <v>0.7</v>
@@ -34803,7 +34803,7 @@
         <v>564</v>
       </c>
       <c r="X415" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y415" s="4">
         <v>0.7</v>
@@ -34880,7 +34880,7 @@
         <v>564</v>
       </c>
       <c r="X416" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y416" s="4">
         <v>0.7</v>
@@ -34957,7 +34957,7 @@
         <v>564</v>
       </c>
       <c r="X417" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y417" s="4">
         <v>0.7</v>
@@ -35034,7 +35034,7 @@
         <v>564</v>
       </c>
       <c r="X418" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y418" s="4">
         <v>0.7</v>
@@ -35111,7 +35111,7 @@
         <v>564</v>
       </c>
       <c r="X419" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y419" s="4">
         <v>0.7</v>
@@ -35188,7 +35188,7 @@
         <v>564</v>
       </c>
       <c r="X420" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y420" s="4">
         <v>0.7</v>
@@ -35265,7 +35265,7 @@
         <v>564</v>
       </c>
       <c r="X421" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y421" s="4">
         <v>0.7</v>
@@ -35342,7 +35342,7 @@
         <v>564</v>
       </c>
       <c r="X422" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y422" s="4">
         <v>0.7</v>
@@ -35419,7 +35419,7 @@
         <v>564</v>
       </c>
       <c r="X423" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y423" s="4">
         <v>0.7</v>
@@ -35496,7 +35496,7 @@
         <v>564</v>
       </c>
       <c r="X424" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y424" s="4">
         <v>0.7</v>
@@ -35573,7 +35573,7 @@
         <v>564</v>
       </c>
       <c r="X425" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y425" s="4">
         <v>0.7</v>
@@ -35650,7 +35650,7 @@
         <v>564</v>
       </c>
       <c r="X426" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y426" s="4">
         <v>0.7</v>
@@ -35727,7 +35727,7 @@
         <v>564</v>
       </c>
       <c r="X427" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y427" s="4">
         <v>0.7</v>
@@ -35804,7 +35804,7 @@
         <v>564</v>
       </c>
       <c r="X428" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y428" s="4">
         <v>0.7</v>
@@ -35881,7 +35881,7 @@
         <v>564</v>
       </c>
       <c r="X429" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y429" s="4">
         <v>0.7</v>
@@ -35958,7 +35958,7 @@
         <v>564</v>
       </c>
       <c r="X430" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y430" s="4">
         <v>0.7</v>
@@ -36035,7 +36035,7 @@
         <v>564</v>
       </c>
       <c r="X431" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y431" s="4">
         <v>0.7</v>
@@ -36112,7 +36112,7 @@
         <v>564</v>
       </c>
       <c r="X432" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y432" s="4">
         <v>0.7</v>
@@ -36189,7 +36189,7 @@
         <v>564</v>
       </c>
       <c r="X433" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y433" s="4">
         <v>0.7</v>
@@ -36266,7 +36266,7 @@
         <v>564</v>
       </c>
       <c r="X434" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y434" s="4">
         <v>0.7</v>
@@ -36343,7 +36343,7 @@
         <v>564</v>
       </c>
       <c r="X435" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y435" s="4">
         <v>0.7</v>
@@ -36420,7 +36420,7 @@
         <v>564</v>
       </c>
       <c r="X436" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y436" s="4">
         <v>0.7</v>
@@ -36497,7 +36497,7 @@
         <v>564</v>
       </c>
       <c r="X437" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y437" s="4">
         <v>0.7</v>
@@ -36574,7 +36574,7 @@
         <v>564</v>
       </c>
       <c r="X438" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y438" s="4">
         <v>0.7</v>
@@ -36651,7 +36651,7 @@
         <v>564</v>
       </c>
       <c r="X439" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y439" s="4">
         <v>0.7</v>
@@ -36728,7 +36728,7 @@
         <v>564</v>
       </c>
       <c r="X440" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y440" s="4">
         <v>0.7</v>
@@ -36805,7 +36805,7 @@
         <v>564</v>
       </c>
       <c r="X441" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y441" s="4">
         <v>0.7</v>
@@ -36882,7 +36882,7 @@
         <v>564</v>
       </c>
       <c r="X442" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y442" s="4">
         <v>0.7</v>
@@ -36959,7 +36959,7 @@
         <v>564</v>
       </c>
       <c r="X443" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y443" s="4">
         <v>0.7</v>
@@ -37036,7 +37036,7 @@
         <v>564</v>
       </c>
       <c r="X444" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y444" s="4">
         <v>0.7</v>
@@ -37113,7 +37113,7 @@
         <v>564</v>
       </c>
       <c r="X445" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y445" s="4">
         <v>0.7</v>
@@ -37190,7 +37190,7 @@
         <v>564</v>
       </c>
       <c r="X446" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y446" s="4">
         <v>0.7</v>
@@ -37267,7 +37267,7 @@
         <v>564</v>
       </c>
       <c r="X447" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y447" s="4">
         <v>0.7</v>
@@ -37344,7 +37344,7 @@
         <v>564</v>
       </c>
       <c r="X448" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y448" s="4">
         <v>0.7</v>
@@ -37421,7 +37421,7 @@
         <v>564</v>
       </c>
       <c r="X449" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y449" s="4">
         <v>0.7</v>
@@ -37498,7 +37498,7 @@
         <v>564</v>
       </c>
       <c r="X450" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y450" s="4">
         <v>0.7</v>
@@ -37575,7 +37575,7 @@
         <v>564</v>
       </c>
       <c r="X451" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y451" s="4">
         <v>0.7</v>
@@ -37652,7 +37652,7 @@
         <v>564</v>
       </c>
       <c r="X452" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y452" s="4">
         <v>0.7</v>
@@ -37729,7 +37729,7 @@
         <v>564</v>
       </c>
       <c r="X453" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y453" s="4">
         <v>0.7</v>
@@ -37806,7 +37806,7 @@
         <v>564</v>
       </c>
       <c r="X454" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y454" s="4">
         <v>0.7</v>
@@ -37883,7 +37883,7 @@
         <v>564</v>
       </c>
       <c r="X455" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y455" s="4">
         <v>0.7</v>
@@ -37960,7 +37960,7 @@
         <v>564</v>
       </c>
       <c r="X456" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y456" s="4">
         <v>0.7</v>
@@ -38037,7 +38037,7 @@
         <v>564</v>
       </c>
       <c r="X457" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y457" s="4">
         <v>0.7</v>
@@ -38114,7 +38114,7 @@
         <v>564</v>
       </c>
       <c r="X458" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y458" s="4">
         <v>0.7</v>
@@ -38191,7 +38191,7 @@
         <v>564</v>
       </c>
       <c r="X459" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y459" s="4">
         <v>0.7</v>
@@ -38268,7 +38268,7 @@
         <v>564</v>
       </c>
       <c r="X460" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y460" s="4">
         <v>0.7</v>
@@ -38345,7 +38345,7 @@
         <v>564</v>
       </c>
       <c r="X461" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y461" s="4">
         <v>0.7</v>
@@ -38422,7 +38422,7 @@
         <v>564</v>
       </c>
       <c r="X462" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y462" s="4">
         <v>0.7</v>
@@ -38499,7 +38499,7 @@
         <v>564</v>
       </c>
       <c r="X463" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y463" s="4">
         <v>0.7</v>
@@ -38576,7 +38576,7 @@
         <v>564</v>
       </c>
       <c r="X464" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y464" s="4">
         <v>0.7</v>
@@ -38653,7 +38653,7 @@
         <v>564</v>
       </c>
       <c r="X465" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y465" s="4">
         <v>0.7</v>
@@ -38730,7 +38730,7 @@
         <v>564</v>
       </c>
       <c r="X466" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y466" s="4">
         <v>0.7</v>
@@ -38807,7 +38807,7 @@
         <v>564</v>
       </c>
       <c r="X467" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y467" s="4">
         <v>0.7</v>
@@ -38884,7 +38884,7 @@
         <v>564</v>
       </c>
       <c r="X468" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y468" s="4">
         <v>0.7</v>
@@ -38961,7 +38961,7 @@
         <v>564</v>
       </c>
       <c r="X469" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y469" s="4">
         <v>0.7</v>
@@ -39038,7 +39038,7 @@
         <v>564</v>
       </c>
       <c r="X470" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y470" s="4">
         <v>0.7</v>
@@ -39115,7 +39115,7 @@
         <v>564</v>
       </c>
       <c r="X471" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y471" s="4">
         <v>0.7</v>
@@ -39192,7 +39192,7 @@
         <v>564</v>
       </c>
       <c r="X472" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y472" s="4">
         <v>0.7</v>
@@ -39269,7 +39269,7 @@
         <v>564</v>
       </c>
       <c r="X473" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y473" s="4">
         <v>0.7</v>
@@ -39346,7 +39346,7 @@
         <v>564</v>
       </c>
       <c r="X474" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y474" s="4">
         <v>0.7</v>
@@ -39423,7 +39423,7 @@
         <v>564</v>
       </c>
       <c r="X475" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y475" s="4">
         <v>0.7</v>
@@ -39500,7 +39500,7 @@
         <v>564</v>
       </c>
       <c r="X476" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y476" s="4">
         <v>0.7</v>
@@ -39577,7 +39577,7 @@
         <v>564</v>
       </c>
       <c r="X477" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y477" s="4">
         <v>0.7</v>
@@ -39654,7 +39654,7 @@
         <v>564</v>
       </c>
       <c r="X478" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y478" s="4">
         <v>0.7</v>
@@ -39731,7 +39731,7 @@
         <v>564</v>
       </c>
       <c r="X479" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y479" s="4">
         <v>0.7</v>
@@ -39808,7 +39808,7 @@
         <v>564</v>
       </c>
       <c r="X480" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y480" s="4">
         <v>0.7</v>
@@ -39885,7 +39885,7 @@
         <v>564</v>
       </c>
       <c r="X481" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y481" s="4">
         <v>0.7</v>
@@ -39962,7 +39962,7 @@
         <v>564</v>
       </c>
       <c r="X482" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y482" s="4">
         <v>0.7</v>
@@ -40039,7 +40039,7 @@
         <v>564</v>
       </c>
       <c r="X483" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y483" s="4">
         <v>0.7</v>
@@ -40116,7 +40116,7 @@
         <v>564</v>
       </c>
       <c r="X484" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y484" s="4">
         <v>0.7</v>
@@ -40193,7 +40193,7 @@
         <v>564</v>
       </c>
       <c r="X485" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y485" s="4">
         <v>0.7</v>
@@ -40270,7 +40270,7 @@
         <v>564</v>
       </c>
       <c r="X486" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y486" s="4">
         <v>0.7</v>
@@ -40347,7 +40347,7 @@
         <v>564</v>
       </c>
       <c r="X487" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y487" s="4">
         <v>0.7</v>
@@ -40424,7 +40424,7 @@
         <v>564</v>
       </c>
       <c r="X488" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y488" s="4">
         <v>0.7</v>
@@ -40501,7 +40501,7 @@
         <v>564</v>
       </c>
       <c r="X489" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y489" s="4">
         <v>0.7</v>
@@ -40578,7 +40578,7 @@
         <v>564</v>
       </c>
       <c r="X490" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y490" s="4">
         <v>0.7</v>
@@ -40655,7 +40655,7 @@
         <v>564</v>
       </c>
       <c r="X491" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y491" s="4">
         <v>0.7</v>
@@ -40732,7 +40732,7 @@
         <v>564</v>
       </c>
       <c r="X492" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y492" s="4">
         <v>0.7</v>
@@ -40809,7 +40809,7 @@
         <v>564</v>
       </c>
       <c r="X493" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y493" s="4">
         <v>0.7</v>
@@ -40886,7 +40886,7 @@
         <v>564</v>
       </c>
       <c r="X494" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y494" s="4">
         <v>0.7</v>
@@ -40963,7 +40963,7 @@
         <v>564</v>
       </c>
       <c r="X495" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y495" s="4">
         <v>0.7</v>
@@ -41040,7 +41040,7 @@
         <v>564</v>
       </c>
       <c r="X496" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y496" s="4">
         <v>0.7</v>
@@ -41117,7 +41117,7 @@
         <v>564</v>
       </c>
       <c r="X497" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y497" s="4">
         <v>0.7</v>
@@ -41194,7 +41194,7 @@
         <v>564</v>
       </c>
       <c r="X498" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y498" s="4">
         <v>0.7</v>
@@ -41271,7 +41271,7 @@
         <v>564</v>
       </c>
       <c r="X499" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y499" s="4">
         <v>0.7</v>
@@ -41348,7 +41348,7 @@
         <v>564</v>
       </c>
       <c r="X500" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y500" s="4">
         <v>0.7</v>
@@ -41425,7 +41425,7 @@
         <v>564</v>
       </c>
       <c r="X501" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y501" s="4">
         <v>0.7</v>
@@ -41502,7 +41502,7 @@
         <v>564</v>
       </c>
       <c r="X502" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y502" s="4">
         <v>0.7</v>
@@ -41579,7 +41579,7 @@
         <v>564</v>
       </c>
       <c r="X503" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y503" s="4">
         <v>0.7</v>
@@ -41656,7 +41656,7 @@
         <v>564</v>
       </c>
       <c r="X504" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y504" s="4">
         <v>0.7</v>
@@ -41733,7 +41733,7 @@
         <v>564</v>
       </c>
       <c r="X505" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y505" s="4">
         <v>0.7</v>
@@ -41810,7 +41810,7 @@
         <v>564</v>
       </c>
       <c r="X506" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y506" s="4">
         <v>0.7</v>
@@ -41887,7 +41887,7 @@
         <v>564</v>
       </c>
       <c r="X507" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y507" s="4">
         <v>0.7</v>
@@ -41964,7 +41964,7 @@
         <v>564</v>
       </c>
       <c r="X508" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y508" s="4">
         <v>0.7</v>
@@ -42041,7 +42041,7 @@
         <v>564</v>
       </c>
       <c r="X509" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y509" s="4">
         <v>0.7</v>
@@ -42118,7 +42118,7 @@
         <v>564</v>
       </c>
       <c r="X510" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y510" s="4">
         <v>0.7</v>
@@ -42195,7 +42195,7 @@
         <v>564</v>
       </c>
       <c r="X511" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y511" s="4">
         <v>0.7</v>
@@ -42272,7 +42272,7 @@
         <v>564</v>
       </c>
       <c r="X512" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y512" s="4">
         <v>0.7</v>
@@ -42349,7 +42349,7 @@
         <v>564</v>
       </c>
       <c r="X513" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y513" s="4">
         <v>0.7</v>
@@ -42426,7 +42426,7 @@
         <v>564</v>
       </c>
       <c r="X514" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y514" s="4">
         <v>0.7</v>
@@ -42503,7 +42503,7 @@
         <v>564</v>
       </c>
       <c r="X515" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y515" s="4">
         <v>0.7</v>
@@ -42580,7 +42580,7 @@
         <v>564</v>
       </c>
       <c r="X516" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y516" s="4">
         <v>0.7</v>
@@ -42657,7 +42657,7 @@
         <v>564</v>
       </c>
       <c r="X517" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y517" s="4">
         <v>0.7</v>
@@ -42734,7 +42734,7 @@
         <v>564</v>
       </c>
       <c r="X518" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y518" s="4">
         <v>0.7</v>
@@ -42811,7 +42811,7 @@
         <v>564</v>
       </c>
       <c r="X519" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y519" s="4">
         <v>0.7</v>
@@ -42888,7 +42888,7 @@
         <v>564</v>
       </c>
       <c r="X520" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y520" s="4">
         <v>0.7</v>
@@ -42965,7 +42965,7 @@
         <v>564</v>
       </c>
       <c r="X521" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y521" s="4">
         <v>0.7</v>
@@ -43042,7 +43042,7 @@
         <v>564</v>
       </c>
       <c r="X522" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y522" s="4">
         <v>0.7</v>
@@ -43119,7 +43119,7 @@
         <v>564</v>
       </c>
       <c r="X523" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y523" s="4">
         <v>0.7</v>
@@ -43196,7 +43196,7 @@
         <v>564</v>
       </c>
       <c r="X524" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y524" s="4">
         <v>0.7</v>
@@ -43273,7 +43273,7 @@
         <v>564</v>
       </c>
       <c r="X525" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y525" s="4">
         <v>0.7</v>
@@ -43350,7 +43350,7 @@
         <v>564</v>
       </c>
       <c r="X526" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y526" s="4">
         <v>0.7</v>
@@ -43427,7 +43427,7 @@
         <v>564</v>
       </c>
       <c r="X527" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y527" s="4">
         <v>0.7</v>
@@ -43504,7 +43504,7 @@
         <v>564</v>
       </c>
       <c r="X528" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y528" s="4">
         <v>0.7</v>
@@ -43581,7 +43581,7 @@
         <v>564</v>
       </c>
       <c r="X529" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y529" s="4">
         <v>0.7</v>
@@ -43658,7 +43658,7 @@
         <v>564</v>
       </c>
       <c r="X530" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y530" s="4">
         <v>0.7</v>
@@ -43735,7 +43735,7 @@
         <v>564</v>
       </c>
       <c r="X531" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y531" s="4">
         <v>0.7</v>
@@ -43812,7 +43812,7 @@
         <v>564</v>
       </c>
       <c r="X532" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y532" s="4">
         <v>0.7</v>
@@ -43889,7 +43889,7 @@
         <v>564</v>
       </c>
       <c r="X533" s="4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="Y533" s="4">
         <v>0.7</v>

</xml_diff>